<commit_message>
Rename libxl and remove files
</commit_message>
<xml_diff>
--- a/shapes.xlsx
+++ b/shapes.xlsx
@@ -57,7 +57,7 @@
     <t>par 6</t>
   </si>
   <si>
-    <t>Cloud</t>
+    <t>Tree</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -442,15 +442,21 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>299</v>
+        <v>90</v>
       </c>
       <c r="C5">
-        <v>399</v>
+        <v>420</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>35</v>
+      </c>
+      <c r="G5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
solved the problem of 2 cells overwriting each other
</commit_message>
<xml_diff>
--- a/shapes.xlsx
+++ b/shapes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="21">
   <si>
     <t>Created by LibXL trial version 4.3.0. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Shape Cout</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Icecream</t>
   </si>
   <si>
     <t>Plane</t>
@@ -123,7 +132,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV5"/>
+  <dimension ref="A1:IV11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -405,7 +414,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -417,7 +426,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -460,30 +469,177 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>810</v>
+        <v>930</v>
       </c>
       <c r="C5">
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>750</v>
+      </c>
+      <c r="C6">
+        <v>240</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>180</v>
+      </c>
+      <c r="C7">
+        <v>360</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>480</v>
+      </c>
+      <c r="C8">
+        <v>360</v>
+      </c>
+      <c r="D8">
         <v>15</v>
       </c>
-      <c r="E5">
+      <c r="E8">
         <v>75</v>
       </c>
-      <c r="F5">
+      <c r="F8">
         <v>50</v>
       </c>
-      <c r="G5">
+      <c r="G8">
         <v>20</v>
       </c>
-      <c r="H5">
+      <c r="H8">
         <v>6</v>
       </c>
-      <c r="I5">
+      <c r="I8">
         <v>6</v>
       </c>
-      <c r="J5">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>360</v>
+      </c>
+      <c r="C9">
+        <v>390</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>630</v>
+      </c>
+      <c r="C10">
+        <v>240</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>690</v>
+      </c>
+      <c r="C11">
+        <v>360</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>150</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>40</v>
+      </c>
+      <c r="H11">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>12</v>
+      </c>
+      <c r="J11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update lives upon refresh
</commit_message>
<xml_diff>
--- a/shapes.xlsx
+++ b/shapes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="22">
   <si>
     <t>Created by LibXL trial version 4.3.0. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -66,16 +66,19 @@
     <t>Shape Cout</t>
   </si>
   <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
     <t>House</t>
   </si>
   <si>
-    <t>Tree</t>
-  </si>
-  <si>
     <t>Icecream</t>
-  </si>
-  <si>
-    <t>Plane</t>
   </si>
 </sst>
 </file>
@@ -409,6 +412,9 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -469,24 +475,15 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>930</v>
+        <v>660</v>
       </c>
       <c r="C5">
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="E5">
-        <v>50</v>
-      </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="G5">
-        <v>50</v>
-      </c>
-      <c r="H5">
         <v>0</v>
       </c>
     </row>
@@ -495,21 +492,27 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>750</v>
+        <v>810</v>
       </c>
       <c r="C6">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E6">
         <v>50</v>
       </c>
       <c r="F6">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6">
         <v>0</v>
       </c>
     </row>
@@ -518,18 +521,21 @@
         <v>19</v>
       </c>
       <c r="B7">
-        <v>180</v>
+        <v>450</v>
       </c>
       <c r="C7">
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="D7">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F7">
+        <v>17</v>
+      </c>
+      <c r="G7">
         <v>0</v>
       </c>
     </row>
@@ -538,30 +544,24 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>480</v>
+        <v>750</v>
       </c>
       <c r="C8">
-        <v>360</v>
+        <v>270</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="E8">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G8">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H8">
-        <v>6</v>
-      </c>
-      <c r="I8">
-        <v>6</v>
-      </c>
-      <c r="J8">
         <v>0</v>
       </c>
     </row>
@@ -570,44 +570,41 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>360</v>
+        <v>1020</v>
       </c>
       <c r="C9">
-        <v>390</v>
+        <v>330</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>50</v>
       </c>
       <c r="F9">
+        <v>17</v>
+      </c>
+      <c r="G9">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>630</v>
+        <v>330</v>
       </c>
       <c r="C10">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
         <v>100</v>
       </c>
-      <c r="E10">
-        <v>50</v>
-      </c>
       <c r="F10">
-        <v>100</v>
-      </c>
-      <c r="G10">
-        <v>50</v>
-      </c>
-      <c r="H10">
         <v>0</v>
       </c>
     </row>
@@ -616,30 +613,24 @@
         <v>20</v>
       </c>
       <c r="B11">
-        <v>690</v>
+        <v>540</v>
       </c>
       <c r="C11">
-        <v>360</v>
+        <v>270</v>
       </c>
       <c r="D11">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E11">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G11">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H11">
-        <v>12</v>
-      </c>
-      <c r="I11">
-        <v>12</v>
-      </c>
-      <c r="J11">
         <v>0</v>
       </c>
     </row>

</xml_diff>